<commit_message>
2-update schedule # and data
</commit_message>
<xml_diff>
--- a/Resources/2-data.xlsx
+++ b/Resources/2-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="34">
   <si>
     <t>CO number</t>
   </si>
@@ -63,7 +63,7 @@
     <t xml:space="preserve">   Sched no</t>
   </si>
   <si>
-    <t>3013696339</t>
+    <t>3013696342</t>
   </si>
   <si>
     <t>TA5TVBPC</t>
@@ -93,28 +93,31 @@
     <t>001</t>
   </si>
   <si>
-    <t>3013696340</t>
-  </si>
-  <si>
-    <t>3013696254</t>
-  </si>
-  <si>
-    <t>TB7SS6AC-0</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>3013696290</t>
-  </si>
-  <si>
-    <t>100317</t>
-  </si>
-  <si>
-    <t>3013696261</t>
-  </si>
-  <si>
-    <t>TB7SS6AC-016</t>
+    <t>3013696343</t>
+  </si>
+  <si>
+    <t>3013696345</t>
+  </si>
+  <si>
+    <t>3013696346</t>
+  </si>
+  <si>
+    <t>3013696347</t>
+  </si>
+  <si>
+    <t>3013696348</t>
+  </si>
+  <si>
+    <t>3013696349</t>
+  </si>
+  <si>
+    <t>3013696350</t>
+  </si>
+  <si>
+    <t>3013696351</t>
+  </si>
+  <si>
+    <t>3013696352</t>
   </si>
 </sst>
 </file>
@@ -460,16 +463,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:N10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" style="3" customWidth="1"/>
     <col min="4" max="4" width="11" style="3" customWidth="1"/>
     <col min="5" max="5" width="6.42578125" style="1" customWidth="1"/>
@@ -627,26 +628,199 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="O4" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="O5" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="O6" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O7" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>17</v>
@@ -682,18 +856,21 @@
         <v>24</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>18</v>
@@ -705,7 +882,7 @@
         <v>20</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>21</v>
@@ -726,15 +903,18 @@
         <v>24</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>17</v>
@@ -770,7 +950,57 @@
         <v>24</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2-add a bunch of data
</commit_message>
<xml_diff>
--- a/Resources/2-data.xlsx
+++ b/Resources/2-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="45">
   <si>
     <t>CO number</t>
   </si>
@@ -109,6 +109,48 @@
   </si>
   <si>
     <t>3013696484</t>
+  </si>
+  <si>
+    <t>3013696525</t>
+  </si>
+  <si>
+    <t>3013696526</t>
+  </si>
+  <si>
+    <t>3013696527</t>
+  </si>
+  <si>
+    <t>3013696528</t>
+  </si>
+  <si>
+    <t>3013696529</t>
+  </si>
+  <si>
+    <t>3013696530</t>
+  </si>
+  <si>
+    <t>3013696532</t>
+  </si>
+  <si>
+    <t>3013696533</t>
+  </si>
+  <si>
+    <t>3013696536</t>
+  </si>
+  <si>
+    <t>3013696537</t>
+  </si>
+  <si>
+    <t>3013696538</t>
+  </si>
+  <si>
+    <t>3013696539</t>
+  </si>
+  <si>
+    <t>3013696540</t>
+  </si>
+  <si>
+    <t>3013696541</t>
   </si>
 </sst>
 </file>
@@ -454,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD5"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,8 +586,12 @@
       <c r="O3" s="2"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -560,9 +606,25 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>28</v>
@@ -583,7 +645,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>28</v>
@@ -603,8 +665,12 @@
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -619,192 +685,324 @@
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
     </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+    </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K12" s="1" t="s">
+      <c r="H16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="N16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K13" s="1" t="s">
+      <c r="H17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="N17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" s="1" t="s">
+      <c r="H18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="M18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O14" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="N18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K15" s="1" t="s">
+      <c r="H19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="M19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O15" s="3" t="s">
-        <v>20</v>
+      <c r="N19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2-update data for PRD test run
</commit_message>
<xml_diff>
--- a/Resources/2-data.xlsx
+++ b/Resources/2-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>CO number</t>
   </si>
@@ -66,16 +66,28 @@
     <t/>
   </si>
   <si>
-    <t>Accessories</t>
-  </si>
-  <si>
-    <t>Bags</t>
-  </si>
-  <si>
-    <t>3013696915</t>
-  </si>
-  <si>
-    <t>3013696916</t>
+    <t>3013997506</t>
+  </si>
+  <si>
+    <t>TA5TVBCC</t>
+  </si>
+  <si>
+    <t>102717</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>EA</t>
+  </si>
+  <si>
+    <t>20-Firm</t>
+  </si>
+  <si>
+    <t>3013992477</t>
+  </si>
+  <si>
+    <t>TB7SX6CC-0</t>
   </si>
 </sst>
 </file>
@@ -442,7 +454,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,158 +524,164 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="A2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="8"/>
+      <c r="A3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="9"/>
       <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
+      <c r="J3" s="8"/>
       <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
       <c r="N3" s="8"/>
-      <c r="O3" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="7" t="s">
+      <c r="O3" s="9"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="9"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="9"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="7" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="9"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="7" t="s">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>18</v>
-      </c>
+      <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -682,9 +700,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>19</v>
-      </c>
+      <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>

</xml_diff>

<commit_message>
2-update data by removing used data, update schedule number
</commit_message>
<xml_diff>
--- a/Resources/2-data.xlsx
+++ b/Resources/2-data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="150" windowWidth="20040" windowHeight="9735"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>CO number</t>
   </si>
@@ -64,12 +64,6 @@
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>3013997506</t>
-  </si>
-  <si>
-    <t>TA5TVBCC</t>
   </si>
   <si>
     <t>102717</t>
@@ -451,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,120 +519,108 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="D2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
+      <c r="G2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="9"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="9" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="5" t="s">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="7" t="s">
         <v>15</v>
       </c>
     </row>
@@ -661,22 +643,22 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="7" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="9" t="s">
         <v>15</v>
       </c>
     </row>
@@ -753,25 +735,6 @@
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
       <c r="O18" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="9" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2A- Updated Script with order entry and Resouse sheet to
</commit_message>
<xml_diff>
--- a/Resources/2-data.xlsx
+++ b/Resources/2-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="20040" windowHeight="9735"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="20040" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
   <si>
     <t>CO number</t>
   </si>
@@ -82,6 +82,120 @@
   </si>
   <si>
     <t>3013992650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer </t>
+  </si>
+  <si>
+    <t>Order type</t>
+  </si>
+  <si>
+    <t>PO</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Delivery Term</t>
+  </si>
+  <si>
+    <t>Delivery Method</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Item Line 1</t>
+  </si>
+  <si>
+    <t>Order Qty</t>
+  </si>
+  <si>
+    <t>Item Line 2</t>
+  </si>
+  <si>
+    <t>Item Line 3</t>
+  </si>
+  <si>
+    <t>Order qty</t>
+  </si>
+  <si>
+    <t>Item Line 4</t>
+  </si>
+  <si>
+    <t>Item Line 5</t>
+  </si>
+  <si>
+    <t>Blanket Agreement</t>
+  </si>
+  <si>
+    <t>Promo</t>
+  </si>
+  <si>
+    <t>Transaction Reason</t>
+  </si>
+  <si>
+    <t>Order count</t>
+  </si>
+  <si>
+    <t>US00025035</t>
+  </si>
+  <si>
+    <t>04B WM Test</t>
+  </si>
+  <si>
+    <t>Stock Balls</t>
+  </si>
+  <si>
+    <t>PPD</t>
+  </si>
+  <si>
+    <t>FXG</t>
+  </si>
+  <si>
+    <t>T2025S</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t>US00025025</t>
+  </si>
+  <si>
+    <t>D75</t>
+  </si>
+  <si>
+    <t>F02</t>
+  </si>
+  <si>
+    <t>US00002914</t>
+  </si>
+  <si>
+    <t>US00025687</t>
+  </si>
+  <si>
+    <t>US00000215</t>
+  </si>
+  <si>
+    <t>F00</t>
+  </si>
+  <si>
+    <t>US00032279</t>
+  </si>
+  <si>
+    <t>F04</t>
+  </si>
+  <si>
+    <t>US00025033</t>
+  </si>
+  <si>
+    <t>FFE</t>
+  </si>
+  <si>
+    <t>US00025282</t>
+  </si>
+  <si>
+    <t>NMF</t>
   </si>
 </sst>
 </file>
@@ -117,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -144,6 +258,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,7 +562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -745,12 +860,349 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2">
+        <v>24</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5">
+        <v>24</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10">
+        <v>504</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11">
+        <v>504</v>
+      </c>
+      <c r="U11">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
2-final pick and update data
</commit_message>
<xml_diff>
--- a/Resources/2-data.xlsx
+++ b/Resources/2-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="88">
   <si>
     <t>CO number</t>
   </si>
@@ -171,91 +171,115 @@
     <t>TA4ACSCUCC-01</t>
   </si>
   <si>
-    <t>3013965909</t>
-  </si>
-  <si>
-    <t>TA1ACFVP-0C</t>
-  </si>
-  <si>
-    <t>092817</t>
-  </si>
-  <si>
-    <t>125.00</t>
-  </si>
-  <si>
-    <t>90</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>3013965750</t>
-  </si>
-  <si>
     <t>TA5TVDFLC</t>
   </si>
   <si>
-    <t>101117</t>
-  </si>
-  <si>
-    <t>30.00</t>
-  </si>
-  <si>
-    <t>3013943720</t>
-  </si>
-  <si>
     <t>TA6ESSP-0C</t>
   </si>
   <si>
-    <t>100217</t>
-  </si>
-  <si>
     <t>4.00</t>
   </si>
   <si>
-    <t>3013970396</t>
-  </si>
-  <si>
     <t>6.00</t>
   </si>
   <si>
-    <t>3013988020</t>
-  </si>
-  <si>
-    <t>092917</t>
-  </si>
-  <si>
-    <t>3013997432</t>
-  </si>
-  <si>
-    <t>111017</t>
-  </si>
-  <si>
-    <t>8.00</t>
-  </si>
-  <si>
-    <t>3013982600</t>
-  </si>
-  <si>
-    <t>TA6ESWDFL-0C</t>
-  </si>
-  <si>
-    <t>101017</t>
-  </si>
-  <si>
-    <t>100.00</t>
-  </si>
-  <si>
-    <t>3013959218</t>
-  </si>
-  <si>
-    <t>TA8PROWDFLSC-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4</t>
-  </si>
-  <si>
-    <t>3013971257</t>
+    <t>TA5ACMFTWLC</t>
+  </si>
+  <si>
+    <t>102517</t>
+  </si>
+  <si>
+    <t>3014006779</t>
+  </si>
+  <si>
+    <t>111717</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>TA5TVWDFLC</t>
+  </si>
+  <si>
+    <t>3013997474</t>
+  </si>
+  <si>
+    <t>TA5TVWRLRC</t>
+  </si>
+  <si>
+    <t>14.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3</t>
+  </si>
+  <si>
+    <t>3013891593</t>
+  </si>
+  <si>
+    <t>TA6ESDFL-0C</t>
+  </si>
+  <si>
+    <t>100317</t>
+  </si>
+  <si>
+    <t>108.00</t>
+  </si>
+  <si>
+    <t>3013996958</t>
+  </si>
+  <si>
+    <t>102617</t>
+  </si>
+  <si>
+    <t>3013992108</t>
+  </si>
+  <si>
+    <t>TA6ESLBP-0C</t>
+  </si>
+  <si>
+    <t>101917</t>
+  </si>
+  <si>
+    <t>3013992654</t>
+  </si>
+  <si>
+    <t>102017</t>
+  </si>
+  <si>
+    <t>3013997376</t>
+  </si>
+  <si>
+    <t>3013991969</t>
+  </si>
+  <si>
+    <t>3013992648</t>
+  </si>
+  <si>
+    <t>3013991970</t>
+  </si>
+  <si>
+    <t>TA7ACDCC-061</t>
+  </si>
+  <si>
+    <t>3013992107</t>
+  </si>
+  <si>
+    <t>102417</t>
+  </si>
+  <si>
+    <t>10.00</t>
+  </si>
+  <si>
+    <t>3013992649</t>
+  </si>
+  <si>
+    <t>3013992652</t>
+  </si>
+  <si>
+    <t>TA7PFZIPC-2</t>
+  </si>
+  <si>
+    <t>TA7PFZIPC-6</t>
   </si>
 </sst>
 </file>
@@ -291,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -307,6 +331,12 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,542 +711,776 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="4" t="s">
+      <c r="A2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="7" t="s">
         <v>21</v>
       </c>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>21</v>
+      <c r="A3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4" s="4" t="s">
+      <c r="A4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="7" t="s">
         <v>21</v>
       </c>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" s="4" t="s">
+      <c r="C5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M5" s="7" t="s">
         <v>21</v>
       </c>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M6" s="4" t="s">
+      <c r="A6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="7" t="s">
         <v>21</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="M7" s="4" t="s">
+      <c r="A7" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M7" s="7" t="s">
         <v>21</v>
       </c>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="A8" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
+      <c r="E8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" s="4"/>
+      <c r="O8" s="5"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="5"/>
+      <c r="A9" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M10" s="4" t="s">
+      <c r="A10" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" s="7" t="s">
         <v>21</v>
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L11" s="4" t="s">
+      <c r="A11" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="M11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
+      <c r="M11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" s="4"/>
+      <c r="O11" s="5"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
+      <c r="A12" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="N12" s="4"/>
       <c r="O12" s="5"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
+      <c r="A13" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="N13" s="4"/>
       <c r="O13" s="5"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
+      <c r="A14" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="N14" s="4"/>
       <c r="O14" s="5"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
+      <c r="A15" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="N15" s="4"/>
       <c r="O15" s="5"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
+      <c r="A16" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="N16" s="4"/>
       <c r="O16" s="5"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
+      <c r="A17" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="N17" s="4"/>
       <c r="O17" s="5"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
+      <c r="A18" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="N18" s="4"/>
       <c r="O18" s="5"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
+      <c r="A19" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="N19" s="4"/>
       <c r="O19" s="5"/>
     </row>
@@ -1304,23 +1568,6 @@
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="5"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>